<commit_message>
Added phonenumber and fixed template
</commit_message>
<xml_diff>
--- a/src/main/resources/ui.replacement/xls/template.xlsx
+++ b/src/main/resources/ui.replacement/xls/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Fulfillment" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="56">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t xml:space="preserve">price.offered_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">price.value</t>
   </si>
   <si>
     <t xml:space="preserve">category_ids[0]</t>
@@ -314,7 +317,7 @@
   </sheetPr>
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
     </sheetView>
   </sheetViews>
@@ -500,10 +503,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -515,19 +518,19 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="15.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="16.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="13.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="16.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="15.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="20.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="25.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="17.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="25.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="17.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="25.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="32.45"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1009" min="22" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="1" width="13.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="16.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="13.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="16.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="15.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="20.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="25.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="17.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="25.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="17.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="25.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="32.45"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1010" min="23" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -574,33 +577,36 @@
         <v>39</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>41</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C2" s="1" t="str">
         <f aca="false">B2</f>
@@ -615,10 +621,10 @@
         <v>Cold Pressed Coconut Oil</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H2" s="1" t="n">
         <v>85</v>
@@ -626,23 +632,23 @@
       <c r="I2" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>46</v>
+      <c r="J2" s="1" t="n">
+        <v>80</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="N2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>49</v>
@@ -661,6 +667,9 @@
       </c>
       <c r="U2" s="1" t="s">
         <v>54</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>